<commit_message>
renewed template with additional column for category
</commit_message>
<xml_diff>
--- a/src/assets/ImportTemplate.xlsx
+++ b/src/assets/ImportTemplate.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>Prompt</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>Clue (optional)</t>
+  </si>
+  <si>
+    <t>Category (names OR ids)</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1177,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1183,7 +1186,8 @@
     <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.6875" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.1328" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3516" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="11" customHeight="1">
@@ -1196,11 +1200,15 @@
       <c r="C1" t="s" s="3">
         <v>2</v>
       </c>
+      <c r="D1" t="s" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" ht="11" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>